<commit_message>
solved De data in de cellen is niet als Tekst gemarkeerd, met de volgende issues:Nummers worden soms anders genoteerd, zoals 4,1E+02. Nummers met volgnummer zoals in "HAAG_01" wordt omgezet naar "HAAG", "1". #641
</commit_message>
<xml_diff>
--- a/tabellen/concept/5.1/objectentabellen/objecten-concept-5.1-SB.xlsx
+++ b/tabellen/concept/5.1/objectentabellen/objecten-concept-5.1-SB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingcrow-my.sharepoint.com/personal/elisabeth_devries_crow_nl/Documents/Documents/GitHub/NLCS/tabellen/concept/5.1/objectentabellen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{E0A2A3EF-5A7D-4926-89BB-683403C988EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{590E082B-725D-4606-A40B-392C83BFA453}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{E0A2A3EF-5A7D-4926-89BB-683403C988EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{328647D3-7DC5-4012-A48F-3CEE83C45EA9}"/>
   <bookViews>
-    <workbookView xWindow="-3015" yWindow="1140" windowWidth="28800" windowHeight="15285" xr2:uid="{EB44BEF5-C594-4473-BA33-0A7E84E11407}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB44BEF5-C594-4473-BA33-0A7E84E11407}"/>
   </bookViews>
   <sheets>
     <sheet name="objecten-concept-5.1-SB" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6182" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6206" uniqueCount="1102">
   <si>
     <t>omschrijving</t>
   </si>
@@ -3302,6 +3302,33 @@
   </si>
   <si>
     <t>*_**_SB_VERKANTING</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>41E1</t>
+  </si>
+  <si>
+    <t>49E1</t>
+  </si>
+  <si>
+    <t>54E1</t>
   </si>
 </sst>
 </file>
@@ -3787,7 +3814,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4165,8 +4192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7C40E0-F10E-48A6-B249-EBCC22134B5F}">
   <dimension ref="A1:BG267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:Y267"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="J1016" sqref="J1016"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,7 +4211,7 @@
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
@@ -4268,7 +4295,7 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -5754,7 +5781,7 @@
       <c r="M12" t="s">
         <v>827</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="1" t="s">
         <v>814</v>
       </c>
       <c r="Y12" t="s">
@@ -6582,7 +6609,7 @@
       <c r="M18" t="s">
         <v>827</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="1" t="s">
         <v>689</v>
       </c>
       <c r="Y18" t="s">
@@ -6725,7 +6752,7 @@
       <c r="M19" t="s">
         <v>827</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="1" t="s">
         <v>679</v>
       </c>
       <c r="Y19" t="s">
@@ -6868,7 +6895,7 @@
       <c r="M20" t="s">
         <v>827</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="1" t="s">
         <v>688</v>
       </c>
       <c r="Y20" t="s">
@@ -7148,7 +7175,7 @@
       <c r="M22" t="s">
         <v>827</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N22" s="1" t="s">
         <v>726</v>
       </c>
       <c r="Y22" t="s">
@@ -7291,7 +7318,7 @@
       <c r="M23" t="s">
         <v>827</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="1" t="s">
         <v>726</v>
       </c>
       <c r="O23" t="s">
@@ -7440,7 +7467,7 @@
       <c r="M24" t="s">
         <v>827</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="1" t="s">
         <v>726</v>
       </c>
       <c r="O24" t="s">
@@ -7589,7 +7616,7 @@
       <c r="M25" t="s">
         <v>827</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="1" t="s">
         <v>726</v>
       </c>
       <c r="O25" t="s">
@@ -7738,7 +7765,7 @@
       <c r="M26" t="s">
         <v>827</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="1" t="s">
         <v>726</v>
       </c>
       <c r="O26" t="s">
@@ -7887,7 +7914,7 @@
       <c r="M27" t="s">
         <v>827</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="1" t="s">
         <v>726</v>
       </c>
       <c r="O27" t="s">
@@ -8036,7 +8063,7 @@
       <c r="M28" t="s">
         <v>827</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="1" t="s">
         <v>726</v>
       </c>
       <c r="O28" t="s">
@@ -8185,7 +8212,7 @@
       <c r="M29" t="s">
         <v>827</v>
       </c>
-      <c r="N29" t="s">
+      <c r="N29" s="1" t="s">
         <v>812</v>
       </c>
       <c r="Y29" t="s">
@@ -8328,7 +8355,7 @@
       <c r="M30" t="s">
         <v>827</v>
       </c>
-      <c r="N30" t="s">
+      <c r="N30" s="1" t="s">
         <v>812</v>
       </c>
       <c r="O30" t="s">
@@ -8477,7 +8504,7 @@
       <c r="M31" t="s">
         <v>827</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="1" t="s">
         <v>812</v>
       </c>
       <c r="O31" t="s">
@@ -8626,7 +8653,7 @@
       <c r="M32" t="s">
         <v>827</v>
       </c>
-      <c r="N32" t="s">
+      <c r="N32" s="1" t="s">
         <v>812</v>
       </c>
       <c r="O32" t="s">
@@ -8775,7 +8802,7 @@
       <c r="M33" t="s">
         <v>827</v>
       </c>
-      <c r="N33" t="s">
+      <c r="N33" s="1" t="s">
         <v>812</v>
       </c>
       <c r="O33" t="s">
@@ -8924,7 +8951,7 @@
       <c r="M34" t="s">
         <v>827</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34" s="1" t="s">
         <v>812</v>
       </c>
       <c r="O34" t="s">
@@ -9073,7 +9100,7 @@
       <c r="M35" t="s">
         <v>827</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N35" s="1" t="s">
         <v>812</v>
       </c>
       <c r="O35" t="s">
@@ -12301,7 +12328,7 @@
       <c r="M59" t="s">
         <v>827</v>
       </c>
-      <c r="N59" t="s">
+      <c r="N59" s="1" t="s">
         <v>806</v>
       </c>
       <c r="Y59" t="s">
@@ -12444,7 +12471,7 @@
       <c r="M60" t="s">
         <v>827</v>
       </c>
-      <c r="N60" t="s">
+      <c r="N60" s="1" t="s">
         <v>806</v>
       </c>
       <c r="O60" t="s">
@@ -12593,7 +12620,7 @@
       <c r="M61" t="s">
         <v>827</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N61" s="1" t="s">
         <v>808</v>
       </c>
       <c r="Y61" t="s">
@@ -12736,7 +12763,7 @@
       <c r="M62" t="s">
         <v>827</v>
       </c>
-      <c r="N62" t="s">
+      <c r="N62" s="1" t="s">
         <v>808</v>
       </c>
       <c r="O62" t="s">
@@ -12885,7 +12912,7 @@
       <c r="M63" t="s">
         <v>827</v>
       </c>
-      <c r="N63" t="s">
+      <c r="N63" s="1" t="s">
         <v>805</v>
       </c>
       <c r="Y63" t="s">
@@ -13028,7 +13055,7 @@
       <c r="M64" t="s">
         <v>827</v>
       </c>
-      <c r="N64" t="s">
+      <c r="N64" s="1" t="s">
         <v>804</v>
       </c>
       <c r="Y64" t="s">
@@ -13171,7 +13198,7 @@
       <c r="M65" t="s">
         <v>827</v>
       </c>
-      <c r="N65" t="s">
+      <c r="N65" s="1" t="s">
         <v>804</v>
       </c>
       <c r="O65" t="s">
@@ -13320,7 +13347,7 @@
       <c r="M66" t="s">
         <v>827</v>
       </c>
-      <c r="N66" t="s">
+      <c r="N66" s="1" t="s">
         <v>807</v>
       </c>
       <c r="Y66" t="s">
@@ -13463,7 +13490,7 @@
       <c r="M67" t="s">
         <v>827</v>
       </c>
-      <c r="N67" t="s">
+      <c r="N67" s="1" t="s">
         <v>807</v>
       </c>
       <c r="O67" t="s">
@@ -13612,7 +13639,7 @@
       <c r="M68" t="s">
         <v>827</v>
       </c>
-      <c r="N68" t="s">
+      <c r="N68" s="1" t="s">
         <v>803</v>
       </c>
       <c r="Y68" t="s">
@@ -13892,7 +13919,7 @@
       <c r="M70" t="s">
         <v>827</v>
       </c>
-      <c r="N70" t="s">
+      <c r="N70" s="1" t="s">
         <v>810</v>
       </c>
       <c r="Y70" t="s">
@@ -14035,7 +14062,7 @@
       <c r="M71" t="s">
         <v>827</v>
       </c>
-      <c r="N71" t="s">
+      <c r="N71" s="1" t="s">
         <v>811</v>
       </c>
       <c r="Y71" t="s">
@@ -15685,7 +15712,7 @@
       <c r="M83" t="s">
         <v>827</v>
       </c>
-      <c r="N83" t="s">
+      <c r="N83" s="1" t="s">
         <v>809</v>
       </c>
       <c r="Y83" t="s">
@@ -18880,8 +18907,8 @@
       <c r="M107" t="s">
         <v>827</v>
       </c>
-      <c r="N107">
-        <v>1</v>
+      <c r="N107" s="1" t="s">
+        <v>1093</v>
       </c>
       <c r="Y107" t="s">
         <v>933</v>
@@ -19023,8 +19050,8 @@
       <c r="M108" t="s">
         <v>827</v>
       </c>
-      <c r="N108">
-        <v>2</v>
+      <c r="N108" s="1" t="s">
+        <v>1094</v>
       </c>
       <c r="Y108" t="s">
         <v>934</v>
@@ -19166,8 +19193,8 @@
       <c r="M109" t="s">
         <v>827</v>
       </c>
-      <c r="N109">
-        <v>3</v>
+      <c r="N109" s="1" t="s">
+        <v>1095</v>
       </c>
       <c r="Y109" t="s">
         <v>935</v>
@@ -19309,8 +19336,8 @@
       <c r="M110" t="s">
         <v>827</v>
       </c>
-      <c r="N110">
-        <v>4</v>
+      <c r="N110" s="1" t="s">
+        <v>1096</v>
       </c>
       <c r="Y110" t="s">
         <v>936</v>
@@ -19452,8 +19479,8 @@
       <c r="M111" t="s">
         <v>827</v>
       </c>
-      <c r="N111">
-        <v>5</v>
+      <c r="N111" s="1" t="s">
+        <v>1097</v>
       </c>
       <c r="Y111" t="s">
         <v>937</v>
@@ -19595,8 +19622,8 @@
       <c r="M112" t="s">
         <v>827</v>
       </c>
-      <c r="N112">
-        <v>6</v>
+      <c r="N112" s="1" t="s">
+        <v>1098</v>
       </c>
       <c r="Y112" t="s">
         <v>938</v>
@@ -20006,8 +20033,8 @@
       <c r="M115" t="s">
         <v>827</v>
       </c>
-      <c r="N115">
-        <v>1</v>
+      <c r="N115" s="1" t="s">
+        <v>1093</v>
       </c>
       <c r="Y115" t="s">
         <v>941</v>
@@ -20149,8 +20176,8 @@
       <c r="M116" t="s">
         <v>827</v>
       </c>
-      <c r="N116">
-        <v>2</v>
+      <c r="N116" s="1" t="s">
+        <v>1094</v>
       </c>
       <c r="Y116" t="s">
         <v>942</v>
@@ -20292,8 +20319,8 @@
       <c r="M117" t="s">
         <v>827</v>
       </c>
-      <c r="N117">
-        <v>3</v>
+      <c r="N117" s="1" t="s">
+        <v>1095</v>
       </c>
       <c r="Y117" t="s">
         <v>943</v>
@@ -20435,8 +20462,8 @@
       <c r="M118" t="s">
         <v>827</v>
       </c>
-      <c r="N118">
-        <v>4</v>
+      <c r="N118" s="1" t="s">
+        <v>1096</v>
       </c>
       <c r="Y118" t="s">
         <v>944</v>
@@ -20578,8 +20605,8 @@
       <c r="M119" t="s">
         <v>827</v>
       </c>
-      <c r="N119">
-        <v>5</v>
+      <c r="N119" s="1" t="s">
+        <v>1097</v>
       </c>
       <c r="Y119" t="s">
         <v>945</v>
@@ -20721,8 +20748,8 @@
       <c r="M120" t="s">
         <v>827</v>
       </c>
-      <c r="N120">
-        <v>6</v>
+      <c r="N120" s="1" t="s">
+        <v>1098</v>
       </c>
       <c r="Y120" t="s">
         <v>946</v>
@@ -21927,7 +21954,7 @@
       <c r="M129" t="s">
         <v>827</v>
       </c>
-      <c r="N129" t="s">
+      <c r="N129" s="1" t="s">
         <v>822</v>
       </c>
       <c r="Y129" t="s">
@@ -22070,7 +22097,7 @@
       <c r="M130" t="s">
         <v>827</v>
       </c>
-      <c r="N130" t="s">
+      <c r="N130" s="1" t="s">
         <v>823</v>
       </c>
       <c r="Y130" t="s">
@@ -23309,7 +23336,7 @@
       <c r="M139" t="s">
         <v>827</v>
       </c>
-      <c r="N139" t="s">
+      <c r="N139" s="1" t="s">
         <v>821</v>
       </c>
       <c r="Y139" t="s">
@@ -23452,7 +23479,7 @@
       <c r="M140" t="s">
         <v>827</v>
       </c>
-      <c r="N140" t="s">
+      <c r="N140" s="1" t="s">
         <v>820</v>
       </c>
       <c r="Y140" t="s">
@@ -23595,7 +23622,7 @@
       <c r="M141" t="s">
         <v>827</v>
       </c>
-      <c r="N141" t="s">
+      <c r="N141" s="1" t="s">
         <v>819</v>
       </c>
       <c r="Y141" t="s">
@@ -26338,7 +26365,7 @@
       <c r="M161" t="s">
         <v>827</v>
       </c>
-      <c r="N161" t="s">
+      <c r="N161" s="1" t="s">
         <v>674</v>
       </c>
       <c r="X161" t="s">
@@ -26624,7 +26651,7 @@
       <c r="M163" t="s">
         <v>827</v>
       </c>
-      <c r="N163" t="s">
+      <c r="N163" s="1" t="s">
         <v>749</v>
       </c>
       <c r="Y163" t="s">
@@ -26767,7 +26794,7 @@
       <c r="M164" t="s">
         <v>827</v>
       </c>
-      <c r="N164" t="s">
+      <c r="N164" s="1" t="s">
         <v>673</v>
       </c>
       <c r="X164" t="s">
@@ -26913,7 +26940,7 @@
       <c r="M165" t="s">
         <v>827</v>
       </c>
-      <c r="N165" t="s">
+      <c r="N165" s="1" t="s">
         <v>672</v>
       </c>
       <c r="X165" t="s">
@@ -27327,7 +27354,7 @@
       <c r="M168" t="s">
         <v>827</v>
       </c>
-      <c r="N168" t="s">
+      <c r="N168" s="1" t="s">
         <v>671</v>
       </c>
       <c r="Y168" t="s">
@@ -27610,7 +27637,7 @@
       <c r="M170" t="s">
         <v>827</v>
       </c>
-      <c r="N170" t="s">
+      <c r="N170" s="1" t="s">
         <v>671</v>
       </c>
       <c r="X170" t="s">
@@ -28164,7 +28191,7 @@
       <c r="M174" t="s">
         <v>827</v>
       </c>
-      <c r="N174" t="s">
+      <c r="N174" s="1" t="s">
         <v>824</v>
       </c>
       <c r="Y174" t="s">
@@ -28307,7 +28334,7 @@
       <c r="M175" t="s">
         <v>827</v>
       </c>
-      <c r="N175" t="s">
+      <c r="N175" s="1" t="s">
         <v>825</v>
       </c>
       <c r="Y175" t="s">
@@ -31050,7 +31077,7 @@
       <c r="M195" t="s">
         <v>827</v>
       </c>
-      <c r="N195" t="s">
+      <c r="N195" s="1" t="s">
         <v>817</v>
       </c>
       <c r="Y195" t="s">
@@ -31470,7 +31497,7 @@
       <c r="M198" t="s">
         <v>827</v>
       </c>
-      <c r="N198" t="s">
+      <c r="N198" s="1" t="s">
         <v>816</v>
       </c>
       <c r="Y198" t="s">
@@ -31613,7 +31640,7 @@
       <c r="M199" t="s">
         <v>827</v>
       </c>
-      <c r="N199" t="s">
+      <c r="N199" s="1" t="s">
         <v>676</v>
       </c>
       <c r="X199" t="s">
@@ -31759,7 +31786,7 @@
       <c r="M200" t="s">
         <v>827</v>
       </c>
-      <c r="N200" t="s">
+      <c r="N200" s="1" t="s">
         <v>815</v>
       </c>
       <c r="Y200" t="s">
@@ -31902,7 +31929,7 @@
       <c r="M201" t="s">
         <v>827</v>
       </c>
-      <c r="N201" t="s">
+      <c r="N201" s="1" t="s">
         <v>677</v>
       </c>
       <c r="X201" t="s">
@@ -32417,8 +32444,8 @@
       <c r="I205" t="s">
         <v>827</v>
       </c>
-      <c r="J205" s="1">
-        <v>410</v>
+      <c r="J205" s="1" t="s">
+        <v>1099</v>
       </c>
       <c r="Y205" t="s">
         <v>1030</v>
@@ -32548,8 +32575,8 @@
       <c r="I206" t="s">
         <v>827</v>
       </c>
-      <c r="J206" s="1">
-        <v>490</v>
+      <c r="J206" s="1" t="s">
+        <v>1100</v>
       </c>
       <c r="Y206" t="s">
         <v>1031</v>
@@ -32810,8 +32837,8 @@
       <c r="I208" t="s">
         <v>827</v>
       </c>
-      <c r="J208" s="1">
-        <v>540</v>
+      <c r="J208" s="1" t="s">
+        <v>1101</v>
       </c>
       <c r="Y208" t="s">
         <v>1033</v>
@@ -34817,8 +34844,8 @@
       <c r="K223" t="s">
         <v>827</v>
       </c>
-      <c r="L223" s="1">
-        <v>410</v>
+      <c r="L223" s="1" t="s">
+        <v>1099</v>
       </c>
       <c r="X223" t="s">
         <v>106</v>
@@ -34957,8 +34984,8 @@
       <c r="K224" t="s">
         <v>827</v>
       </c>
-      <c r="L224" s="1">
-        <v>490</v>
+      <c r="L224" s="1" t="s">
+        <v>1100</v>
       </c>
       <c r="X224" t="s">
         <v>103</v>
@@ -35234,8 +35261,8 @@
       <c r="K226" t="s">
         <v>827</v>
       </c>
-      <c r="L226" s="1">
-        <v>540</v>
+      <c r="L226" s="1" t="s">
+        <v>1101</v>
       </c>
       <c r="Y226" t="s">
         <v>1051</v>
@@ -36476,8 +36503,8 @@
       <c r="K235" t="s">
         <v>827</v>
       </c>
-      <c r="L235" s="1">
-        <v>410</v>
+      <c r="L235" s="1" t="s">
+        <v>1099</v>
       </c>
       <c r="X235" t="s">
         <v>106</v>
@@ -36616,8 +36643,8 @@
       <c r="K236" t="s">
         <v>827</v>
       </c>
-      <c r="L236" s="1">
-        <v>490</v>
+      <c r="L236" s="1" t="s">
+        <v>1100</v>
       </c>
       <c r="X236" t="s">
         <v>103</v>
@@ -36893,8 +36920,8 @@
       <c r="K238" t="s">
         <v>827</v>
       </c>
-      <c r="L238" s="1">
-        <v>540</v>
+      <c r="L238" s="1" t="s">
+        <v>1101</v>
       </c>
       <c r="Y238" t="s">
         <v>1063</v>
@@ -39195,8 +39222,8 @@
       <c r="K255" t="s">
         <v>827</v>
       </c>
-      <c r="L255" s="1">
-        <v>410</v>
+      <c r="L255" s="1" t="s">
+        <v>1099</v>
       </c>
       <c r="Y255" t="s">
         <v>1080</v>
@@ -39332,8 +39359,8 @@
       <c r="K256" t="s">
         <v>827</v>
       </c>
-      <c r="L256" s="1">
-        <v>490</v>
+      <c r="L256" s="1" t="s">
+        <v>1100</v>
       </c>
       <c r="Y256" t="s">
         <v>1081</v>
@@ -39606,8 +39633,8 @@
       <c r="K258" t="s">
         <v>827</v>
       </c>
-      <c r="L258" s="1">
-        <v>540</v>
+      <c r="L258" s="1" t="s">
+        <v>1101</v>
       </c>
       <c r="Y258" t="s">
         <v>1083</v>

</xml_diff>